<commit_message>
Packet Nuget ScottPlot installé
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B1BE75-A0FC-41DF-B80A-7C3B702A27B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5817749F-937C-4062-A214-0C0970F41FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -131,6 +131,15 @@
   </si>
   <si>
     <t xml:space="preserve">Création des user et technical stories </t>
+  </si>
+  <si>
+    <t>Recherche du type de donnée (Voir technical Stories)</t>
+  </si>
+  <si>
+    <t>Explication projet par M.Carrel</t>
+  </si>
+  <si>
+    <t>Création d'un graphe</t>
   </si>
 </sst>
 </file>
@@ -1051,13 +1060,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6.9444444444444441E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1.0416666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1069,7 +1078,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1980,9 +1989,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2035,7 +2044,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 0 heurs 0 minutes</v>
+        <v>0 jours 2 heurs 55 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2050,15 +2059,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2101,7 +2110,9 @@
         <v>45534</v>
       </c>
       <c r="C7" s="44"/>
-      <c r="D7" s="45"/>
+      <c r="D7" s="45">
+        <v>15</v>
+      </c>
       <c r="E7" s="46" t="s">
         <v>6</v>
       </c>
@@ -2111,15 +2122,23 @@
       <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="str">
+      <c r="A8" s="8">
         <f>IF(ISBLANK(B8),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B8))</f>
-        <v/>
-      </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="48"/>
+        <v>35</v>
+      </c>
+      <c r="B8" s="47">
+        <v>45534</v>
+      </c>
+      <c r="C8" s="48">
+        <v>1</v>
+      </c>
       <c r="D8" s="49"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="37"/>
+      <c r="E8" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>30</v>
+      </c>
       <c r="G8" s="16"/>
       <c r="M8" t="s">
         <v>3</v>
@@ -2132,15 +2151,25 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="str">
+      <c r="A9" s="17">
         <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B9))</f>
-        <v/>
-      </c>
-      <c r="B9" s="51"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="37"/>
+        <v>35</v>
+      </c>
+      <c r="B9" s="51">
+        <v>45534</v>
+      </c>
+      <c r="C9" s="52">
+        <v>1</v>
+      </c>
+      <c r="D9" s="53">
+        <v>30</v>
+      </c>
+      <c r="E9" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>31</v>
+      </c>
       <c r="G9" s="18"/>
       <c r="M9" t="s">
         <v>4</v>
@@ -2153,15 +2182,23 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="str">
+      <c r="A10" s="8">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v/>
-      </c>
-      <c r="B10" s="47"/>
+        <v>35</v>
+      </c>
+      <c r="B10" s="47">
+        <v>45534</v>
+      </c>
       <c r="C10" s="48"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="37"/>
+      <c r="D10" s="49">
+        <v>10</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>32</v>
+      </c>
       <c r="G10" s="16"/>
       <c r="M10" t="s">
         <v>5</v>
@@ -8601,7 +8638,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8609,7 +8646,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0</v>
+        <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8637,7 +8674,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C7" s="28" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8645,7 +8682,7 @@
       </c>
       <c r="D7" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8701,7 +8738,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C11" s="40" t="str">
         <f>'Journal de travail'!M15</f>
@@ -8709,7 +8746,7 @@
       </c>
       <c r="D11" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -8718,7 +8755,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0</v>
+        <v>3.8194444444444448E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8955,6 +8992,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -8963,15 +9009,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8994,6 +9031,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9002,12 +9047,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
refactor Scatter multiple oke
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C350A09-CBF5-4AB0-9345-54B45A067240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D6BB85-7882-40C4-9FED-7E58FFFD858E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="4590" yWindow="1215" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>Refactorisation du tableau "nbPoint" en liste (factorisation nécessitant l'ajout d'une methode pour passer les valeur de la liste dans un tableau pour l'affichage du graph)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refactorisation du code du graphe afin qu'il puisse afficher plusieur équipes </t>
   </si>
 </sst>
 </file>
@@ -1084,7 +1087,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.11805555555555555</c:v>
+                  <c:v>0.1388888888888889</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2015,7 +2018,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2068,7 +2071,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 6 heurs 9 minutes</v>
+        <v>0 jours 6 heurs 40 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2087,11 +2090,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>190</v>
+        <v>220</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>370</v>
+        <v>400</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2449,15 +2452,23 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="str">
+      <c r="A19" s="17">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="51"/>
+        <v>37</v>
+      </c>
+      <c r="B19" s="51">
+        <v>45548</v>
+      </c>
       <c r="C19" s="52"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="37"/>
+      <c r="D19" s="53">
+        <v>30</v>
+      </c>
+      <c r="E19" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="37" t="s">
+        <v>41</v>
+      </c>
       <c r="G19" s="18"/>
       <c r="O19">
         <v>55</v>
@@ -8726,7 +8737,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8734,7 +8745,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.11805555555555555</v>
+        <v>0.1388888888888889</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8843,7 +8854,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.1736111111111111</v>
+        <v>0.19444444444444445</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9080,6 +9091,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9088,15 +9108,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9119,6 +9130,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9127,12 +9146,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Chore: Journal de travail
Mise à jour du journal de travail
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5BDF6D-4CBE-4197-B8CD-4D4BB87FFCE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F93D16-380A-412D-86B6-52714A95E5C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="1215" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t xml:space="preserve">Appel a une api oke </t>
+  </si>
+  <si>
+    <t>Absence</t>
+  </si>
+  <si>
+    <t>Discussion avec le prof sur l'evolution du métier</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1117,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.125E-2</c:v>
+                  <c:v>3.8194444444444448E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2024,7 +2030,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2077,7 +2083,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 7 heurs 30 minutes</v>
+        <v>0 jours 10 heurs 40 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2092,15 +2098,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>450</v>
+        <v>640</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2521,27 +2527,43 @@
       <c r="G21" s="18"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="str">
+      <c r="A22" s="8">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="47"/>
-      <c r="C22" s="48"/>
+        <v>38</v>
+      </c>
+      <c r="B22" s="47">
+        <v>45555</v>
+      </c>
+      <c r="C22" s="48">
+        <v>3</v>
+      </c>
       <c r="D22" s="49"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="37"/>
+      <c r="E22" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="37" t="s">
+        <v>44</v>
+      </c>
       <c r="G22" s="16"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="str">
+      <c r="A23" s="17">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="51"/>
+        <v>39</v>
+      </c>
+      <c r="B23" s="51">
+        <v>45562</v>
+      </c>
       <c r="C23" s="52"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="37"/>
+      <c r="D23" s="53">
+        <v>10</v>
+      </c>
+      <c r="E23" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="37" t="s">
+        <v>45</v>
+      </c>
       <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -8859,7 +8881,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C11" s="40" t="str">
         <f>'Journal de travail'!M15</f>
@@ -8867,7 +8889,7 @@
       </c>
       <c r="D11" s="34">
         <f t="shared" si="0"/>
-        <v>3.125E-2</v>
+        <v>3.8194444444444448E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -8876,7 +8898,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.22916666666666666</v>
+        <v>0.2361111111111111</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9113,15 +9135,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9130,6 +9143,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9152,14 +9174,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9168,4 +9182,12 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Doc: Update du journal de travail
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F93D16-380A-412D-86B6-52714A95E5C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A909169D-547F-4CA9-A478-A2AE6D1528E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>Discussion avec le prof sur l'evolution du métier</t>
+  </si>
+  <si>
+    <t>Ajout d'un fichier CSV contenant les données des équipes</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1102,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1736111111111111</c:v>
+                  <c:v>0.19791666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2030,7 +2033,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2083,7 +2086,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 10 heurs 40 minutes</v>
+        <v>0 jours 11 heurs 15 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2102,11 +2105,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>280</v>
+        <v>315</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>640</v>
+        <v>675</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2567,15 +2570,23 @@
       <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="str">
+      <c r="A24" s="8">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v/>
-      </c>
-      <c r="B24" s="47"/>
+        <v>39</v>
+      </c>
+      <c r="B24" s="47">
+        <v>45562</v>
+      </c>
       <c r="C24" s="48"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="37"/>
+      <c r="D24" s="49">
+        <v>35</v>
+      </c>
+      <c r="E24" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="37" t="s">
+        <v>46</v>
+      </c>
       <c r="G24" s="16"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -8781,7 +8792,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>190</v>
+        <v>225</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8789,7 +8800,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.1736111111111111</v>
+        <v>0.19791666666666666</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8898,7 +8909,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.2361111111111111</v>
+        <v>0.26041666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9135,6 +9146,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9143,15 +9163,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9174,6 +9185,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9182,12 +9201,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Chore: Mise à jour du journal de travail
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A909169D-547F-4CA9-A478-A2AE6D1528E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F759E1AA-6B62-4F5B-ACC9-64236B6BF6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>Ajout d'un fichier CSV contenant les données des équipes</t>
+  </si>
+  <si>
+    <t>Ajout de la methode getAllTeams qui permet de récupéer toutes les équipe de la nba en lisant le fichier CSV</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1105,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19791666666666666</c:v>
+                  <c:v>0.22569444444444445</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2033,7 +2036,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F29:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2086,7 +2089,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 11 heurs 15 minutes</v>
+        <v>0 jours 11 heurs 55 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2105,11 +2108,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>315</v>
+        <v>355</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>675</v>
+        <v>715</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2589,16 +2592,24 @@
       </c>
       <c r="G24" s="16"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="str">
+    <row r="25" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="17">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="51"/>
+        <v>39</v>
+      </c>
+      <c r="B25" s="51">
+        <v>45562</v>
+      </c>
       <c r="C25" s="52"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="37"/>
+      <c r="D25" s="53">
+        <v>40</v>
+      </c>
+      <c r="E25" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>47</v>
+      </c>
       <c r="G25" s="18"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -8792,7 +8803,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8800,7 +8811,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.19791666666666666</v>
+        <v>0.22569444444444445</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8909,7 +8920,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.26041666666666663</v>
+        <v>0.28819444444444442</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9146,15 +9157,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9163,6 +9165,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9185,14 +9196,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9201,4 +9204,12 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Feat: Ajout  de la methode getTeamsStats
Ajout de la méthode getTeamsStats qui permet de créer un objet de la classe Team ayant le nom et la liste des score de l'équipe pour l'entièreté de la saison
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F759E1AA-6B62-4F5B-ACC9-64236B6BF6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5612B41E-2D6E-42F0-8EE5-066FEF60BA7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>Ajout de la methode getAllTeams qui permet de récupéer toutes les équipe de la nba en lisant le fichier CSV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout de la methode getTeamsStats qui permet de récupérer pour chaque équipe NBA leur statistique pour la saison </t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1108,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22569444444444445</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2036,7 +2039,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F29:F30"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2089,7 +2092,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 11 heurs 55 minutes</v>
+        <v>0 jours 12 heurs 30 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2108,11 +2111,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>355</v>
+        <v>390</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>715</v>
+        <v>750</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2612,16 +2615,24 @@
       </c>
       <c r="G25" s="18"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="str">
+    <row r="26" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
-        <v/>
-      </c>
-      <c r="B26" s="47"/>
+        <v>39</v>
+      </c>
+      <c r="B26" s="47">
+        <v>45562</v>
+      </c>
       <c r="C26" s="48"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="37"/>
+      <c r="D26" s="49">
+        <v>35</v>
+      </c>
+      <c r="E26" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="37" t="s">
+        <v>48</v>
+      </c>
       <c r="G26" s="16"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -8803,7 +8814,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>265</v>
+        <v>300</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8811,7 +8822,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.22569444444444445</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8920,7 +8931,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.28819444444444442</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9157,6 +9168,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9165,15 +9185,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9196,6 +9207,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9204,12 +9223,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Doc: MIse a jour journal de travail
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5612B41E-2D6E-42F0-8EE5-066FEF60BA7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F67AE90-C720-47D8-9469-252B183CA6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ajout de la methode getTeamsStats qui permet de récupérer pour chaque équipe NBA leur statistique pour la saison </t>
+  </si>
+  <si>
+    <t>Essaie de conversion de la date en string du CSV en format numéros du jour de la semaine ()</t>
   </si>
 </sst>
 </file>
@@ -1108,7 +1111,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25</c:v>
+                  <c:v>0.27777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2092,7 +2095,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 12 heurs 30 minutes</v>
+        <v>0 jours 13 heurs 10 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2111,11 +2114,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>390</v>
+        <v>430</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>750</v>
+        <v>790</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2636,15 +2639,23 @@
       <c r="G26" s="16"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="str">
+      <c r="A27" s="17">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
-        <v/>
-      </c>
-      <c r="B27" s="51"/>
+        <v>39</v>
+      </c>
+      <c r="B27" s="51">
+        <v>45562</v>
+      </c>
       <c r="C27" s="52"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="37"/>
+      <c r="D27" s="53">
+        <v>40</v>
+      </c>
+      <c r="E27" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="37" t="s">
+        <v>49</v>
+      </c>
       <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -8814,7 +8825,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>300</v>
+        <v>340</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8822,7 +8833,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.25</v>
+        <v>0.27777777777777779</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8931,7 +8942,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.3125</v>
+        <v>0.34027777777777779</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9168,15 +9179,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9185,6 +9187,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9207,14 +9218,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9223,4 +9226,12 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Feat: Récupération d'une liste d'équipe
Récupération d'une liste d'équipe ainsi que ses scores ses score et la date du score respectif
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F67AE90-C720-47D8-9469-252B183CA6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87622EFF-04EF-410D-98EC-AE0B00B39603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="31500" yWindow="3345" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>Essaie de conversion de la date en string du CSV en format numéros du jour de la semaine ()</t>
+  </si>
+  <si>
+    <t>Récupération dans une liste d'équipe l'équipe ainsi que son score et le jour du match</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1114,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.27777777777777779</c:v>
+                  <c:v>0.3298611111111111</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2041,8 +2044,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2095,7 +2098,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 13 heurs 10 minutes</v>
+        <v>0 jours 14 heurs 25 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2110,15 +2113,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>430</v>
+        <v>445</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>790</v>
+        <v>865</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2659,15 +2662,25 @@
       <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="str">
+      <c r="A28" s="8">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v/>
-      </c>
-      <c r="B28" s="47"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="36"/>
+        <v>40</v>
+      </c>
+      <c r="B28" s="47">
+        <v>45568</v>
+      </c>
+      <c r="C28" s="48">
+        <v>1</v>
+      </c>
+      <c r="D28" s="49">
+        <v>15</v>
+      </c>
+      <c r="E28" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="36" t="s">
+        <v>50</v>
+      </c>
       <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -8821,11 +8834,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>340</v>
+        <v>355</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8833,7 +8846,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.27777777777777779</v>
+        <v>0.3298611111111111</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8942,7 +8955,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.34027777777777779</v>
+        <v>0.39236111111111105</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9179,6 +9192,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9187,15 +9209,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9218,6 +9231,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9226,12 +9247,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Doc: Mise à jour du journal de travail
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87622EFF-04EF-410D-98EC-AE0B00B39603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3528E4E-B0C4-474E-BE98-BE9F7C2614A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="31500" yWindow="3345" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Récupération dans une liste d'équipe l'équipe ainsi que son score et le jour du match</t>
+  </si>
+  <si>
+    <t>M.Carrel nous a donné des feedback sur l'avancé des projets (Besoin d'avancer sur la documentation)</t>
   </si>
 </sst>
 </file>
@@ -1123,7 +1126,7 @@
                   <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.472222222222222E-3</c:v>
+                  <c:v>1.3888888888888888E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2044,8 +2047,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2098,7 +2101,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 14 heurs 25 minutes</v>
+        <v>0 jours 14 heurs 40 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2117,11 +2120,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>445</v>
+        <v>460</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>865</v>
+        <v>880</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2684,15 +2687,23 @@
       <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="str">
+      <c r="A29" s="17">
         <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B29))</f>
-        <v/>
-      </c>
-      <c r="B29" s="51"/>
+        <v>40</v>
+      </c>
+      <c r="B29" s="51">
+        <v>45569</v>
+      </c>
       <c r="C29" s="52"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="36"/>
+      <c r="D29" s="53">
+        <v>15</v>
+      </c>
+      <c r="E29" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="36" t="s">
+        <v>51</v>
+      </c>
       <c r="G29" s="18"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -8892,7 +8903,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C8" s="29" t="str">
         <f>'Journal de travail'!M12</f>
@@ -8900,7 +8911,7 @@
       </c>
       <c r="D8" s="34">
         <f t="shared" si="0"/>
-        <v>3.472222222222222E-3</v>
+        <v>1.3888888888888888E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -8955,7 +8966,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.39236111111111105</v>
+        <v>0.40277777777777779</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9192,15 +9203,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9209,6 +9211,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9231,14 +9242,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9247,4 +9250,12 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc: Mise à jour journal de travail
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB61F70A-FF88-4B01-BA3C-5FA8ADD1035B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7F7595-90BB-4753-9D11-B2D699B13417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>Fix de la méthode GetTeamStructure (Bug: La séléction des données était éronnée et attribuait le score de l'équipe à domicil si l'équipe jouait à l'extérieur)</t>
+  </si>
+  <si>
+    <t>Feat: Affichage des ligne pour chaque équipe sur le graphe</t>
   </si>
 </sst>
 </file>
@@ -383,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -510,11 +513,89 @@
     <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -683,80 +764,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1120,7 +1127,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.33680555555555558</c:v>
+                  <c:v>0.37152777777777779</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1844,18 +1851,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="14">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2050,8 +2057,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <pane ySplit="6" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2104,7 +2111,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 14 heurs 50 minutes</v>
+        <v>0 jours 15 heurs 40 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2123,11 +2130,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>470</v>
+        <v>520</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>890</v>
+        <v>940</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2730,15 +2737,23 @@
       <c r="G30" s="16"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="str">
+      <c r="A31" s="17">
         <f>IF(ISBLANK(B31),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B31))</f>
-        <v/>
-      </c>
-      <c r="B31" s="51"/>
+        <v>40</v>
+      </c>
+      <c r="B31" s="51">
+        <v>45569</v>
+      </c>
       <c r="C31" s="52"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="36"/>
+      <c r="D31" s="53">
+        <v>50</v>
+      </c>
+      <c r="E31" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="36" t="s">
+        <v>53</v>
+      </c>
       <c r="G31" s="18"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -2750,7 +2765,7 @@
       <c r="C32" s="48"/>
       <c r="D32" s="49"/>
       <c r="E32" s="50"/>
-      <c r="F32" s="37"/>
+      <c r="F32" s="57"/>
       <c r="G32" s="16"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -8760,28 +8775,28 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E532">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
       <formula>$E7="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8860,7 +8875,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>365</v>
+        <v>415</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8868,7 +8883,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.33680555555555558</v>
+        <v>0.37152777777777779</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8977,7 +8992,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.40972222222222221</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Doc: mise à jour journal travail
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7F7595-90BB-4753-9D11-B2D699B13417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2251FA2D-E3EA-4784-965E-9F27128D0ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>Feat: Affichage des ligne pour chaque équipe sur le graphe</t>
+  </si>
+  <si>
+    <t>Création US</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +1127,7 @@
                 <c:formatCode>hh\ "h"\ mm\ "min"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>4.1666666666666664E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.37152777777777779</c:v>
@@ -2058,7 +2061,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2111,7 +2114,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 15 heurs 40 minutes</v>
+        <v>0 jours 16 heurs 39 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2126,7 +2129,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>420</v>
+        <v>480</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
@@ -2134,7 +2137,7 @@
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>940</v>
+        <v>1000</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2757,15 +2760,23 @@
       <c r="G31" s="18"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="str">
+      <c r="A32" s="8">
         <f>IF(ISBLANK(B32),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B32))</f>
-        <v/>
-      </c>
-      <c r="B32" s="47"/>
-      <c r="C32" s="48"/>
+        <v>40</v>
+      </c>
+      <c r="B32" s="47">
+        <v>45569</v>
+      </c>
+      <c r="C32" s="48">
+        <v>1</v>
+      </c>
       <c r="D32" s="49"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="57"/>
+      <c r="E32" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="57" t="s">
+        <v>54</v>
+      </c>
       <c r="G32" s="16"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -8853,7 +8864,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C4,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B4">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C4,'Journal de travail'!$D$7:$D$532)</f>
@@ -8865,7 +8876,7 @@
       </c>
       <c r="D4" s="34">
         <f>(A4+B4)/1440</f>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -8992,7 +9003,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.44444444444444442</v>
+        <v>0.48611111111111116</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Doc: Update journal travail
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2251FA2D-E3EA-4784-965E-9F27128D0ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46785901-E282-42BD-840D-D4FB1C5C0E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>Création US</t>
+  </si>
+  <si>
+    <t>Mise à jour VS</t>
   </si>
 </sst>
 </file>
@@ -509,6 +512,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -516,89 +523,11 @@
     <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -767,6 +696,80 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1148,7 +1151,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.8194444444444448E-2</c:v>
+                  <c:v>5.9027777777777776E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1854,18 +1857,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2061,7 +2064,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2096,11 +2099,11 @@
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
       <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
@@ -2114,7 +2117,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 16 heurs 39 minutes</v>
+        <v>0 jours 17 heurs 10 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2133,20 +2136,20 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>520</v>
+        <v>550</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>1000</v>
+        <v>1030</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="1:15" s="21" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
@@ -2774,21 +2777,29 @@
       <c r="E32" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="57" t="s">
+      <c r="F32" s="55" t="s">
         <v>54</v>
       </c>
       <c r="G32" s="16"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="str">
+      <c r="A33" s="17">
         <f>IF(ISBLANK(B33),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B33))</f>
-        <v/>
-      </c>
-      <c r="B33" s="51"/>
+        <v>40</v>
+      </c>
+      <c r="B33" s="51">
+        <v>45570</v>
+      </c>
       <c r="C33" s="52"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="36"/>
+      <c r="D33" s="53">
+        <v>30</v>
+      </c>
+      <c r="E33" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33" s="36" t="s">
+        <v>55</v>
+      </c>
       <c r="G33" s="18"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -8786,28 +8797,28 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E532">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>$E7="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8986,7 +8997,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="C11" s="40" t="str">
         <f>'Journal de travail'!M15</f>
@@ -8994,7 +9005,7 @@
       </c>
       <c r="D11" s="34">
         <f t="shared" si="0"/>
-        <v>3.8194444444444448E-2</v>
+        <v>5.9027777777777776E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -9003,7 +9014,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.48611111111111116</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9240,6 +9251,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9248,15 +9268,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9279,6 +9290,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9287,12 +9306,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc: update journal de travail
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7D58BD-C0F6-44A6-A9E2-53AEF76E9F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9DD9FD-CD5C-4E98-9AAE-68BA42C21C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -211,7 +211,10 @@
     <t>Mise à jour VS</t>
   </si>
   <si>
-    <t>Tentaive de rendre les legendes cliquable (Non réussite)</t>
+    <t>Tentative de rendre les legendes cliquable (Non réussite)</t>
+  </si>
+  <si>
+    <t>Feat: Mise en place du filtre par équipe</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1139,7 @@
                   <c:v>4.1666666666666664E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.38541666666666669</c:v>
+                  <c:v>0.46875</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2067,7 +2070,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2120,7 +2123,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 17 heurs 30 minutes</v>
+        <v>0 jours 19 heurs 30 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2135,7 +2138,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>480</v>
+        <v>600</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
@@ -2143,7 +2146,7 @@
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>1050</v>
+        <v>1170</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2826,15 +2829,23 @@
       <c r="G34" s="16"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="str">
+      <c r="A35" s="17">
         <f>IF(ISBLANK(B35),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B35))</f>
-        <v/>
-      </c>
-      <c r="B35" s="51"/>
-      <c r="C35" s="52"/>
+        <v>40</v>
+      </c>
+      <c r="B35" s="51">
+        <v>45570</v>
+      </c>
+      <c r="C35" s="52">
+        <v>2</v>
+      </c>
       <c r="D35" s="53"/>
-      <c r="E35" s="54"/>
-      <c r="F35" s="37"/>
+      <c r="E35" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="37" t="s">
+        <v>57</v>
+      </c>
       <c r="G35" s="18"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -8904,7 +8915,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
@@ -8916,7 +8927,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.38541666666666669</v>
+        <v>0.46875</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -9025,7 +9036,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.52083333333333337</v>
+        <v>0.60416666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Doc: Mise à jour Journal travail + commencement du rapport
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEF2179-8B79-4CF7-80EB-933644236049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64A5A39-EE17-4069-BD4E-32E1E95B7652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="4590" yWindow="1215" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t xml:space="preserve">Revue/correction des user stories </t>
+  </si>
+  <si>
+    <t>Le prof nous a présenter IceTools</t>
   </si>
 </sst>
 </file>
@@ -1154,7 +1157,7 @@
                   <c:v>2.7777777777777776E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0833333333333332E-2</c:v>
+                  <c:v>3.125E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2076,7 +2079,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2129,7 +2132,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 19 heurs 49 minutes</v>
+        <v>0 jours 20 heurs 5 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2148,11 +2151,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>590</v>
+        <v>605</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>1190</v>
+        <v>1205</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2895,15 +2898,23 @@
       <c r="G37" s="18"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="str">
+      <c r="A38" s="8">
         <f>IF(ISBLANK(B38),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B38))</f>
-        <v/>
-      </c>
-      <c r="B38" s="47"/>
+        <v>41</v>
+      </c>
+      <c r="B38" s="47">
+        <v>45576</v>
+      </c>
       <c r="C38" s="48"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="36"/>
+      <c r="D38" s="49">
+        <v>15</v>
+      </c>
+      <c r="E38" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="36" t="s">
+        <v>60</v>
+      </c>
       <c r="G38" s="16"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -8995,7 +9006,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C8" s="29" t="str">
         <f>'Journal de travail'!M12</f>
@@ -9003,7 +9014,7 @@
       </c>
       <c r="D8" s="34">
         <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -9058,7 +9069,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.61805555555555558</v>
+        <v>0.62847222222222221</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Doc: Updarte journal de travail
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64A5A39-EE17-4069-BD4E-32E1E95B7652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23B2A5F-BE33-40B9-B808-7BFDAE4995A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="1215" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="3540" yWindow="3135" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="62">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -225,6 +225,9 @@
   <si>
     <t>Le prof nous a présenter IceTools</t>
   </si>
+  <si>
+    <t>Ecriture de l'introduction de l'analyse prélininaire du rapport</t>
+  </si>
 </sst>
 </file>
 
@@ -238,7 +241,7 @@
     <numFmt numFmtId="168" formatCode="00\ &quot;min&quot;"/>
     <numFmt numFmtId="169" formatCode="hh\ &quot;h&quot;\ mm\ &quot;min&quot;"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -316,6 +319,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -407,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -537,6 +546,10 @@
     </xf>
     <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1154,7 +1167,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7777777777777776E-2</c:v>
+                  <c:v>3.125E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3.125E-2</c:v>
@@ -2079,7 +2092,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
+      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2132,7 +2145,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 20 heurs 5 minutes</v>
+        <v>0 jours 20 heurs 10 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2151,11 +2164,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>1205</v>
+        <v>1210</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2917,16 +2930,24 @@
       </c>
       <c r="G38" s="16"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="str">
+    <row r="39" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="17">
         <f>IF(ISBLANK(B39),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B39))</f>
-        <v/>
-      </c>
-      <c r="B39" s="51"/>
+        <v>41</v>
+      </c>
+      <c r="B39" s="51">
+        <v>45576</v>
+      </c>
       <c r="C39" s="52"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="54"/>
-      <c r="F39" s="36"/>
+      <c r="D39" s="53">
+        <v>5</v>
+      </c>
+      <c r="E39" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39" s="58" t="s">
+        <v>61</v>
+      </c>
       <c r="G39" s="18"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -8988,7 +9009,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C7" s="28" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8996,7 +9017,7 @@
       </c>
       <c r="D7" s="34">
         <f t="shared" si="0"/>
-        <v>2.7777777777777776E-2</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -9069,7 +9090,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.62847222222222221</v>
+        <v>0.63194444444444442</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Doc: Updates journal de travail
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/Docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BILEL\Documents\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E02C0B1-7B57-4F34-9928-F228DE72BCEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA9214F-A626-4FD2-B868-B6F03F582A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="70">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>Refactore: (Graph.cs) Mise en place du flowLayoutPanel dans la conception</t>
+  </si>
+  <si>
+    <t>Doc: (DataSelection.cs) Ajout des commentaires dans la classe DataSelection.cs</t>
   </si>
 </sst>
 </file>
@@ -1182,7 +1185,7 @@
                   <c:v>4.1666666666666664E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.49652777777777779</c:v>
+                  <c:v>0.50694444444444442</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2113,7 +2116,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F50" sqref="F50"/>
+      <selection pane="bottomLeft" activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2166,7 +2169,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 21 heurs 54 minutes</v>
+        <v>0 jours 22 heurs 10 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2185,11 +2188,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>715</v>
+        <v>730</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>1315</v>
+        <v>1330</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -3097,7 +3100,7 @@
         <v>41</v>
       </c>
       <c r="B46" s="47">
-        <v>45576</v>
+        <v>45578</v>
       </c>
       <c r="C46" s="48"/>
       <c r="D46" s="49">
@@ -3112,15 +3115,23 @@
       <c r="G46" s="16"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A47" s="17" t="str">
+      <c r="A47" s="17">
         <f>IF(ISBLANK(B47),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B47))</f>
-        <v/>
-      </c>
-      <c r="B47" s="51"/>
+        <v>41</v>
+      </c>
+      <c r="B47" s="51">
+        <v>45578</v>
+      </c>
       <c r="C47" s="52"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="54"/>
-      <c r="F47" s="36"/>
+      <c r="D47" s="53">
+        <v>15</v>
+      </c>
+      <c r="E47" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47" s="36" t="s">
+        <v>69</v>
+      </c>
       <c r="G47" s="18"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.5">
@@ -9050,7 +9061,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>475</v>
+        <v>490</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -9058,7 +9069,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.49652777777777779</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -9167,7 +9178,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.70486111111111105</v>
+        <v>0.71527777777777768</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -9181,26 +9192,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9423,10 +9414,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9443,20 +9465,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>